<commit_message>
10th - Bug Fixes & Tickers Update
</commit_message>
<xml_diff>
--- a/Reports/MarketBeatRank/TanzyToInvest/AMMA.xlsx
+++ b/Reports/MarketBeatRank/TanzyToInvest/AMMA.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="35">
   <si>
     <t>Jun_10</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>Jun_17</t>
+  </si>
+  <si>
+    <t>Jun_26</t>
+  </si>
+  <si>
+    <t>Benchmark</t>
+  </si>
+  <si>
+    <t>Evercore ISI</t>
   </si>
 </sst>
 </file>
@@ -144,8 +153,36 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -160,20 +197,24 @@
   <cols>
     <col min="3" max="3" customWidth="true" width="8.0" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="8.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="8.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>0</v>
       </c>
     </row>
@@ -193,6 +234,9 @@
       <c r="E2" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -210,6 +254,9 @@
       <c r="E3" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F3" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -227,6 +274,9 @@
       <c r="E4" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F4" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -244,6 +294,9 @@
       <c r="E5" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F5" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -261,6 +314,9 @@
       <c r="E6" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F6" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -278,6 +334,9 @@
       <c r="E7" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F7" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -295,6 +354,9 @@
       <c r="E8" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F8" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -312,6 +374,9 @@
       <c r="E9" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F9" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -329,6 +394,9 @@
       <c r="E10" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F10" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -346,6 +414,9 @@
       <c r="E11" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F11" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -363,6 +434,9 @@
       <c r="E12" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F12" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -380,6 +454,9 @@
       <c r="E13" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F13" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -397,6 +474,9 @@
       <c r="E14" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F14" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -414,6 +494,9 @@
       <c r="E15" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F15" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -431,6 +514,9 @@
       <c r="E16" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F16" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
@@ -448,6 +534,9 @@
       <c r="E17" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F17" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -465,6 +554,9 @@
       <c r="E18" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F18" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -482,6 +574,9 @@
       <c r="E19" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F19" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -499,6 +594,9 @@
       <c r="E20" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F20" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
@@ -516,6 +614,9 @@
       <c r="E21" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F21" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
@@ -533,6 +634,9 @@
       <c r="E22" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F22" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -550,6 +654,9 @@
       <c r="E23" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F23" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
@@ -567,6 +674,9 @@
       <c r="E24" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F24" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
@@ -584,6 +694,9 @@
       <c r="E25" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F25" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
@@ -601,6 +714,9 @@
       <c r="E26" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F26" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
@@ -616,6 +732,25 @@
         <v>2</v>
       </c>
       <c r="E27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>